<commit_message>
add charts for snmt vs unmt
</commit_message>
<xml_diff>
--- a/snmt-vs-unmt/scores-all.xlsx
+++ b/snmt-vs-unmt/scores-all.xlsx
@@ -1,20 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tg/work/papers/007-mt-eval-macro/snmt-vs-unmt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{57A8D1CD-F5EA-F242-B432-6D781BA25C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A17438-FFDA-D14F-84B1-DB4490985F43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1600" windowWidth="40560" windowHeight="21300"/>
+    <workbookView xWindow="5840" yWindow="1680" windowWidth="40560" windowHeight="21300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scores-all" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'scores-all'!$A$13:$A$18</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'scores-all'!$B$11:$B$12</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'scores-all'!$B$13:$B$18</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'scores-all'!$C$11:$C$12</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'scores-all'!$C$13:$C$18</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'scores-all'!$D$11:$D$12</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'scores-all'!$D$13:$D$18</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'scores-all'!$E$11:$E$12</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'scores-all'!$E$13:$E$18</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">'scores-all'!$B$11:$B$12</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">'scores-all'!$B$13:$B$18</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">'scores-all'!$C$11:$C$12</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">'scores-all'!$C$13:$C$18</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">'scores-all'!$D$11:$D$12</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">'scores-all'!$D$13:$D$18</definedName>
+    <definedName name="_xlchart.v2.16" hidden="1">'scores-all'!$E$11:$E$12</definedName>
+    <definedName name="_xlchart.v2.17" hidden="1">'scores-all'!$E$13:$E$18</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">'scores-all'!$A$13:$A$18</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
   <si>
     <t>DEEN</t>
   </si>
@@ -77,14 +97,20 @@
   <si>
     <t>$\Delta$</t>
   </si>
+  <si>
+    <t>SNMT</t>
+  </si>
+  <si>
+    <t>UNMT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -563,13 +589,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -626,6 +653,1581 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>SNMT and UNMT</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> performance using BLEU and MacroF1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.1634707487665139E-2"/>
+          <c:y val="0.19743702299627752"/>
+          <c:w val="0.9250538802841084"/>
+          <c:h val="0.72138216754826978"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'scores-all'!$B$11:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>BLEU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SNMT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4345484448139413E-2"/>
+                  <c:y val="8.1743860440701647E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.9659277800871774E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.586371112034845E-3"/>
+                  <c:y val="4.0871930220351196E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.172742224069821E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0759113336104534E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'scores-all'!$A$13:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>DEEN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ENDE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FREN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ENFR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ROEN</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ENRO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'scores-all'!$B$13:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'scores-all'!$C$11:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>BLEU</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UNMT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'scores-all'!$A$13:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>DEEN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ENDE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FREN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ENFR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ROEN</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ENRO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'scores-all'!$C$13:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>33.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'scores-all'!$D$11:$D$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>MacroF1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SNMT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2874688755776266E-17"/>
+                  <c:y val="-2.4523158132210794E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'scores-all'!$A$13:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>DEEN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ENDE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FREN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ENFR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ROEN</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ENRO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'scores-all'!$D$13:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'scores-all'!$E$11:$E$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>MacroF1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UNMT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'scores-all'!$A$13:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>DEEN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ENDE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FREN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ENFR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ROEN</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ENRO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'scores-all'!$E$13:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>33.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AD4C-AA41-A2AE-F0BDCD0B02FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="68402304"/>
+        <c:axId val="69108880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="68402304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69108880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69108880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="68402304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22375185813558404"/>
+          <c:y val="0.10655076876877451"/>
+          <c:w val="0.60629170921364151"/>
+          <c:h val="6.88521802368183E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>71965</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>516467</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3BA0706-B5DE-1A41-B2DC-96A7C1857DC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -924,11 +2526,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:S8"/>
+      <selection activeCell="A11" sqref="A11:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1411,8 +3013,352 @@
         <v>6.4793000000000003E-2</v>
       </c>
     </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="S11" s="4"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C13" s="2">
+        <v>33.9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>33.6</v>
+      </c>
+      <c r="F13" s="2">
+        <v>58.7</v>
+      </c>
+      <c r="G13" s="2">
+        <v>57.9</v>
+      </c>
+      <c r="H13" s="2">
+        <v>59.9</v>
+      </c>
+      <c r="I13" s="2">
+        <v>58</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.21088599999999999</v>
+      </c>
+      <c r="K13" s="1">
+        <v>-2.5899999999999999E-2</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.285279</v>
+      </c>
+      <c r="M13" s="1">
+        <v>6.7020999999999997E-2</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>47.7</v>
+      </c>
+      <c r="G14" s="2">
+        <v>48.1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>53.3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>52</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-0.133607</v>
+      </c>
+      <c r="K14" s="1">
+        <v>-0.204261</v>
+      </c>
+      <c r="L14" s="1">
+        <v>-0.11151800000000001</v>
+      </c>
+      <c r="M14" s="1">
+        <v>-0.19675200000000001</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>31.1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>41.6</v>
+      </c>
+      <c r="E15" s="2">
+        <v>33.6</v>
+      </c>
+      <c r="F15" s="2">
+        <v>60.5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>58.3</v>
+      </c>
+      <c r="H15" s="2">
+        <v>59.1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>57.3</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.182093</v>
+      </c>
+      <c r="K15" s="1">
+        <v>6.5627000000000005E-2</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.243144</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.153669</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2">
+        <v>25.6</v>
+      </c>
+      <c r="C16" s="2">
+        <v>27.1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>31.9</v>
+      </c>
+      <c r="E16" s="2">
+        <v>27.3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>53</v>
+      </c>
+      <c r="G16" s="2">
+        <v>52.3</v>
+      </c>
+      <c r="H16" s="2">
+        <v>56</v>
+      </c>
+      <c r="I16" s="2">
+        <v>57.7</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.103988</v>
+      </c>
+      <c r="K16" s="1">
+        <v>4.1993000000000003E-2</v>
+      </c>
+      <c r="L16" s="1">
+        <v>9.5728999999999995E-2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>6.3386999999999999E-2</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>30.8</v>
+      </c>
+      <c r="C17" s="2">
+        <v>29.6</v>
+      </c>
+      <c r="D17" s="2">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="E17" s="2">
+        <v>33</v>
+      </c>
+      <c r="F17" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="G17" s="2">
+        <v>56.5</v>
+      </c>
+      <c r="H17" s="2">
+        <v>58</v>
+      </c>
+      <c r="I17" s="2">
+        <v>54.7</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4.0400000000000002E-3</v>
+      </c>
+      <c r="K17" s="1">
+        <v>-5.7596000000000001E-2</v>
+      </c>
+      <c r="L17" s="1">
+        <v>4.5012000000000003E-2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>-4.37E-4</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>31</v>
+      </c>
+      <c r="D18" s="2">
+        <v>34.6</v>
+      </c>
+      <c r="E18" s="2">
+        <v>31</v>
+      </c>
+      <c r="F18" s="2">
+        <v>55.4</v>
+      </c>
+      <c r="G18" s="2">
+        <v>53.4</v>
+      </c>
+      <c r="H18" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="I18" s="2">
+        <v>56.7</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3.0152000000000002E-2</v>
+      </c>
+      <c r="K18" s="1">
+        <v>-4.5825999999999999E-2</v>
+      </c>
+      <c r="L18" s="1">
+        <v>2.6971999999999999E-2</v>
+      </c>
+      <c r="M18" s="1">
+        <v>-3.7821E-2</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="S18" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
@@ -1422,5 +3368,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>